<commit_message>
Production files v2.0: BoM list update
</commit_message>
<xml_diff>
--- a/HW/Product/V2.0/BoM/PIC32DevKit.xlsx
+++ b/HW/Product/V2.0/BoM/PIC32DevKit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\SAMPI\P32DK\HW\Product\V2.0\BoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851D163F-ADF7-4CD4-B95E-48D3C88584DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD3C65B-C173-4D40-A5F0-4CAF1D4AFBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-780" windowWidth="20730" windowHeight="11760" xr2:uid="{D0AE83A9-3369-4B79-919F-2A4E075B35E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="136">
   <si>
     <t>Quantity</t>
   </si>
@@ -48,15 +48,9 @@
     <t>Unit Cost</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>R11</t>
   </si>
   <si>
-    <t>R15</t>
-  </si>
-  <si>
     <t>R17</t>
   </si>
   <si>
@@ -141,60 +135,6 @@
     <t>Manufacture</t>
   </si>
   <si>
-    <t>0603_RES, 5k1</t>
-  </si>
-  <si>
-    <t>0603_RES, 1k</t>
-  </si>
-  <si>
-    <t>0603_RES, 52k3</t>
-  </si>
-  <si>
-    <t>0603_RES, 10k</t>
-  </si>
-  <si>
-    <t>0603_RES, 2k2</t>
-  </si>
-  <si>
-    <t>0603_RES, 4k7</t>
-  </si>
-  <si>
-    <t>0603_RES, 100k</t>
-  </si>
-  <si>
-    <t>0603_RES, 12k</t>
-  </si>
-  <si>
-    <t>SOT563_DIODE, AP6220X</t>
-  </si>
-  <si>
-    <t>UQFN28_0.4X4X4, PIC32MM0XXXGPM028</t>
-  </si>
-  <si>
-    <t>TQFP64-10X10X1, PIC32MM0XXXGPM064</t>
-  </si>
-  <si>
-    <t>SOT143, PRTR5V0U2X,215</t>
-  </si>
-  <si>
-    <t>DTFN1212-6LD-PL-1, MIC5528</t>
-  </si>
-  <si>
-    <t>QFN50P400X400X100-25N-D, USB2422</t>
-  </si>
-  <si>
-    <t>SOP50P310X100-8N, LEVEL SHIFTER</t>
-  </si>
-  <si>
-    <t>SOIC8_3.9_5.3, SPI FLASH</t>
-  </si>
-  <si>
-    <t>SOIC8_3.9_5.3, SPI EEPROM</t>
-  </si>
-  <si>
-    <t>SOT-23-3-AP2210, RZF013P01TL</t>
-  </si>
-  <si>
     <t>SML-D12U8W, BLED</t>
   </si>
   <si>
@@ -334,6 +274,174 @@
   </si>
   <si>
     <t>CAP CER 10PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-51-kohm-0603-1</t>
+  </si>
+  <si>
+    <t>RES 5.1K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-075K1L</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-1-kohm-0603-5</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603JR-131KL</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-53-6-kohm-0603-1</t>
+  </si>
+  <si>
+    <t>RES 53.6K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-0753K6L</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>AC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-10-kohm-0603-1-</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-2-2-kohm-0603-5</t>
+  </si>
+  <si>
+    <t>RES 2.2K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603JR-072K2L</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-4-7-kohm-0603-5</t>
+  </si>
+  <si>
+    <t>R3, R15</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 5% 1/10W 060</t>
+  </si>
+  <si>
+    <t>RC0603JR-074K7L</t>
+  </si>
+  <si>
+    <t>RC0603FR-0712KL</t>
+  </si>
+  <si>
+    <t>RES 12K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-12-kohm-0603-1-</t>
+  </si>
+  <si>
+    <t>AP62201Z6-7</t>
+  </si>
+  <si>
+    <t>DCDC CONV HV BUCK SOT563 T&amp;R 3K</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/AP62201Z6-7/13161377</t>
+  </si>
+  <si>
+    <t>PIC32MM0064GPM028-I/M6</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 64KB FLASH 28UQFN</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/PIC32MM0064GPM028-I-M6/8037777</t>
+  </si>
+  <si>
+    <t>PIC32MM0256GPM064T-I/PT</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 256KB FLASH 64TQFP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/PIC32MM0256GPM064T-I-PT/7354645</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/DRTR5V0U2SR-7/4402528</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.5VWM SOT143</t>
+  </si>
+  <si>
+    <t>DRTR5V0U2SR-7</t>
+  </si>
+  <si>
+    <t>MIC5528-3.3YMX-TR</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 500MA 6XTDFN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/MIC5528-3-3YMX-TR/4465358</t>
+  </si>
+  <si>
+    <t>USB2422/MJ</t>
+  </si>
+  <si>
+    <t>IC HUB CTLR USB 2.0 24QFN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/USB2422-MJ/4080182</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/74AVC2T45DC-125/1692558</t>
+  </si>
+  <si>
+    <t>74AVC2T45DC,125</t>
+  </si>
+  <si>
+    <t>IC TRNSLTR BIDIRECTIONAL 8VSSOP</t>
+  </si>
+  <si>
+    <t>Nexperia</t>
+  </si>
+  <si>
+    <t>SST25PF080B-80-4C-SAE-T</t>
+  </si>
+  <si>
+    <t>IC FLASH 8MBIT SPI 80MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/SST25PF080B-80-4C-SAE-T/3908714</t>
+  </si>
+  <si>
+    <t>25AA160D-I/SN</t>
+  </si>
+  <si>
+    <t>IC EEPROM 16KBIT SPI 10MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/25AA160D-I-SN/2125494</t>
+  </si>
+  <si>
+    <t>RZF013P01TL</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 12V 1.3A TUMT3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/RZF013P01TL/5042831</t>
   </si>
 </sst>
 </file>
@@ -343,7 +451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$VND]\ #,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +485,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,7 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,7 +573,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -777,43 +894,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5033DA-B212-4008-848D-3BC8E84D6B52}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -825,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,19 +951,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="G2" s="6">
         <v>8</v>
@@ -863,19 +981,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G3" s="6">
         <v>21</v>
@@ -884,7 +1002,7 @@
         <v>207</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I41" si="0">G3*H3</f>
+        <f t="shared" ref="I3:I40" si="0">G3*H3</f>
         <v>4347</v>
       </c>
     </row>
@@ -893,19 +1011,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="G4" s="6">
         <v>2</v>
@@ -923,19 +1041,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="G5" s="6">
         <v>3</v>
@@ -953,19 +1071,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G6" s="6">
         <v>4</v>
@@ -982,14 +1100,20 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="F7" s="12" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G7" s="6">
         <v>4</v>
@@ -1004,14 +1128,20 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="F8" s="12" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G8" s="6">
         <v>3</v>
@@ -1026,17 +1156,23 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="12"/>
+        <v>88</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="F9" s="12" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="G9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7">
@@ -1048,14 +1184,20 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="12"/>
+        <v>90</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="F10" s="12" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="G10" s="6">
         <v>10</v>
@@ -1070,14 +1212,20 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>93</v>
+      </c>
       <c r="F11" s="12" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="G11" s="6">
         <v>5</v>
@@ -1092,14 +1240,20 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="F12" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
@@ -1112,16 +1266,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="D13" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="F13" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="6">
         <v>1</v>
@@ -1134,16 +1294,22 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="D14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>106</v>
+      </c>
       <c r="F14" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
@@ -1156,16 +1322,22 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="D15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="F15" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="6">
         <v>1</v>
@@ -1178,16 +1350,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="D16" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>113</v>
+      </c>
       <c r="F16" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="6">
         <v>1</v>
@@ -1200,16 +1378,22 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="D17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="12"/>
+        <v>115</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>114</v>
+      </c>
       <c r="F17" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" s="6">
         <v>1</v>
@@ -1222,19 +1406,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="D18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="12"/>
+        <v>118</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="F18" s="12" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="G18" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7">
@@ -1244,19 +1434,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="D19" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="12"/>
+        <v>121</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F19" s="12" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="G19" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7">
@@ -1266,16 +1462,22 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="D20" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="12"/>
+        <v>125</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>123</v>
+      </c>
       <c r="F20" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" s="6">
         <v>1</v>
@@ -1288,21 +1490,27 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="D21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="12"/>
+        <v>128</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="F21" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21" s="6">
         <v>1</v>
       </c>
-      <c r="H21" s="7"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1310,16 +1518,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="D22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="12"/>
+        <v>131</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="F22" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="6">
         <v>1</v>
@@ -1332,21 +1546,27 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="D23" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="12"/>
+        <v>134</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="F23" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="6">
         <v>1</v>
       </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1354,16 +1574,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="6">
         <v>1</v>
@@ -1376,19 +1596,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G25" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7">
@@ -1398,19 +1618,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="12" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="G26" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7">
@@ -1420,16 +1640,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="12" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" s="6">
         <v>1</v>
@@ -1442,16 +1662,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="12" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G28" s="6">
         <v>1</v>
@@ -1464,19 +1684,19 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="12" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="G29" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7">
@@ -1486,19 +1706,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="12" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="G30" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7">
@@ -1508,16 +1728,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="12" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" s="6">
         <v>1</v>
@@ -1530,19 +1750,19 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="12" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="G32" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7">
@@ -1552,19 +1772,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="12" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G33" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7">
@@ -1574,16 +1794,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="12" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G34" s="6">
         <v>1</v>
@@ -1596,16 +1816,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="12" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="6">
         <v>1</v>
@@ -1618,16 +1838,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="12" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G36" s="6">
         <v>1</v>
@@ -1640,16 +1860,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="12" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37" s="6">
         <v>1</v>
@@ -1662,16 +1882,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="12" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G38" s="6">
         <v>1</v>
@@ -1684,16 +1904,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="12" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G39" s="6">
         <v>1</v>
@@ -1706,16 +1926,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="12" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G40" s="6">
         <v>1</v>
@@ -1727,44 +1947,22 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>40</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" s="6">
-        <v>1</v>
-      </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="9">
-        <f>SUM(G2:G41)</f>
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="9">
+        <f>SUM(G2:G40)</f>
         <v>96</v>
       </c>
-      <c r="H42" s="10">
-        <f>I42/G42</f>
+      <c r="H41" s="10">
+        <f>I41/G41</f>
         <v>185.57291666666666</v>
       </c>
-      <c r="I42" s="10">
-        <f>SUM(I2:I41)</f>
+      <c r="I41" s="10">
+        <f>SUM(I2:I40)</f>
         <v>17815</v>
       </c>
     </row>
@@ -1776,11 +1974,28 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{D5F25149-DC80-4BEC-92E8-E789439A3874}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{BC2B10D5-BF73-438A-92A4-F1EAE5931FED}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{DF914C99-8A25-4884-A22A-E4C5140CF07D}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{422863BC-F505-4FFA-88D2-ECD707A30A19}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{44022EB2-CD12-4DE9-9DDE-9EDF232292DA}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{45DA230D-C55E-4F7A-BAC9-F0E1B819468B}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{FC4E87AF-9803-4BE3-B91D-E8C5F288ECD3}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{89AE6C98-46B4-4829-95D8-2BE291DDEF45}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{E4FC1D59-4DA0-49F7-9685-C9AECA06C100}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{C6088598-7E76-4AFF-BA80-92CCF303B6AE}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{2CD2DA28-7B5E-4C02-8822-FBD83B316B8D}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{B9D46221-E16E-4461-9AEE-268C0CE7A6F7}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{7D59F71F-DC69-4F60-B5F7-B985A8889484}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{25555BB1-8503-4902-8D28-49B76EAF7381}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{E3501AB6-E97B-409C-B24B-DD0DB03176C0}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{07ADFDFD-D8C3-42C7-AFCB-42E20CBB5868}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{A006401B-D073-44F6-89A8-300FF5B79CCC}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{49E01FA6-C108-4308-AD2C-DAE45DB62021}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{C1FA9CE7-CDAF-4E38-A7A5-5512E7BED9CF}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{4B8B16CD-A2B2-46EF-BEBD-F0DB4520BFC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
   <ignoredErrors>
-    <ignoredError sqref="H42" formula="1"/>
+    <ignoredError sqref="H41" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>